<commit_message>
fix(condo): DOMA-8315 fixed export of property meters readings
</commit_message>
<xml_diff>
--- a/apps/condo/domains/meter/templates/PropertyMeterReadingsExportTemplate.xlsx
+++ b/apps/condo/domains/meter/templates/PropertyMeterReadingsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>{d.i18n.date}</t>
   </si>
@@ -19,9 +19,6 @@
     <t>{d.i18n.address}</t>
   </si>
   <si>
-    <t>{d.i18n.accountNumber}</t>
-  </si>
-  <si>
     <t>{d.i18n.resource}</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>{d.meter[i].address}</t>
   </si>
   <si>
-    <t>{d.meter[i].accountNumber}</t>
-  </si>
-  <si>
     <t>{d.meter[i].resource}</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t>{d.meter[i + 1].address}</t>
-  </si>
-  <si>
-    <t>{d.meter[i + 1].accountNumber}</t>
   </si>
   <si>
     <t>{d.meter[i + 1].resource}</t>
@@ -1377,7 +1368,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1385,12 +1376,11 @@
   <cols>
     <col min="1" max="1" width="15.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3516" style="1" customWidth="1"/>
-    <col min="6" max="9" width="19.1719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.3516" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3516" style="1" customWidth="1"/>
+    <col min="5" max="8" width="19.1719" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.3516" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1421,72 +1411,63 @@
       <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="D2" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="E2" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="F2" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="G2" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="H2" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="I2" t="s" s="2">
         <v>17</v>
-      </c>
-      <c r="I2" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>19</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="D3" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="E3" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="F3" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="G3" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="F3" t="s" s="2">
+      <c r="H3" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="G3" t="s" s="2">
+      <c r="I3" t="s" s="2">
         <v>26</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s" s="2">
-        <v>29</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
@@ -1498,8 +1479,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" s="6"/>
@@ -1510,8 +1490,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" s="6"/>
@@ -1522,8 +1501,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" s="6"/>
@@ -1534,8 +1512,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1546,8 +1523,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1558,8 +1534,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="9"/>
@@ -1570,8 +1545,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>